<commit_message>
echoMRI editions and cd1 exploration
</commit_message>
<xml_diff>
--- a/data/echoMRI/Kotz04292025.xlsx
+++ b/data/echoMRI/Kotz04292025.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10125"/>
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Documents/GitHub/data/data/echoMRI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F81EC8C-2FB3-6D43-B5D3-0A1E290D3EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E75371-9D1B-6F43-9BE7-9F28F5A2D1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="44800" windowHeight="25200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtractedScans" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ExtractedScans!$A$1:$J$25</definedName>
     <definedName name="ExtractedScans">ExtractedScans!$A$1:$J$25</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
@@ -157,9 +158,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,7 +467,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -505,7 +505,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
@@ -534,7 +534,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
@@ -563,7 +563,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
@@ -1176,7 +1176,7 @@
         <v>43</v>
       </c>
       <c r="B25">
-        <v>9363</v>
+        <v>9362</v>
       </c>
       <c r="C25">
         <v>1.31</v>

</xml_diff>